<commit_message>
Commit on 17 Mar 2023
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_UBSExcel/Test-data/KUBSTestData.xlsx
+++ b/AzentioAutomationFramework_UBSExcel/Test-data/KUBSTestData.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4091" uniqueCount="1401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4454" uniqueCount="1536">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -4243,6 +4243,411 @@
   </si>
   <si>
     <t>2527</t>
+  </si>
+  <si>
+    <t>TABLE_CHAIRS_42676</t>
+  </si>
+  <si>
+    <t>2528</t>
+  </si>
+  <si>
+    <t>FIXTURESANDFITTINGS1-TABLESANDCHAIRS01-TABLE_CHAIRS_42676</t>
+  </si>
+  <si>
+    <t>8625</t>
+  </si>
+  <si>
+    <t>2227</t>
+  </si>
+  <si>
+    <t>ITEM1962221391</t>
+  </si>
+  <si>
+    <t>5088</t>
+  </si>
+  <si>
+    <t>FIXTURESANDFITTINGS1-TABLESANDCHAIRS01-TABLE_CHAIRS_42676_AZENTMAIN_2001</t>
+  </si>
+  <si>
+    <t>114074</t>
+  </si>
+  <si>
+    <t>ITEM1512191215</t>
+  </si>
+  <si>
+    <t>5090</t>
+  </si>
+  <si>
+    <t>5091</t>
+  </si>
+  <si>
+    <t>114077</t>
+  </si>
+  <si>
+    <t>ITEM1872121224</t>
+  </si>
+  <si>
+    <t>5093</t>
+  </si>
+  <si>
+    <t>5094</t>
+  </si>
+  <si>
+    <t>5095</t>
+  </si>
+  <si>
+    <t>114081</t>
+  </si>
+  <si>
+    <t>ITEM1612861415</t>
+  </si>
+  <si>
+    <t>5097</t>
+  </si>
+  <si>
+    <t>5098</t>
+  </si>
+  <si>
+    <t>114084</t>
+  </si>
+  <si>
+    <t>ITEM1822281138</t>
+  </si>
+  <si>
+    <t>5100</t>
+  </si>
+  <si>
+    <t>5101</t>
+  </si>
+  <si>
+    <t>114087</t>
+  </si>
+  <si>
+    <t>ITEM1512341283</t>
+  </si>
+  <si>
+    <t>5103</t>
+  </si>
+  <si>
+    <t>NITM107241</t>
+  </si>
+  <si>
+    <t>114089</t>
+  </si>
+  <si>
+    <t>114090</t>
+  </si>
+  <si>
+    <t>ITEM1842071272</t>
+  </si>
+  <si>
+    <t>5106</t>
+  </si>
+  <si>
+    <t>5107</t>
+  </si>
+  <si>
+    <t>114093</t>
+  </si>
+  <si>
+    <t>ITEM1362921479</t>
+  </si>
+  <si>
+    <t>5109</t>
+  </si>
+  <si>
+    <t>114095</t>
+  </si>
+  <si>
+    <t>114096</t>
+  </si>
+  <si>
+    <t>ITEM1262221033</t>
+  </si>
+  <si>
+    <t>5112</t>
+  </si>
+  <si>
+    <t>5113</t>
+  </si>
+  <si>
+    <t>114107</t>
+  </si>
+  <si>
+    <t>TABLE_CHAIRS_36981</t>
+  </si>
+  <si>
+    <t>2547</t>
+  </si>
+  <si>
+    <t>FIXTURESANDFITTINGS1-TABLESANDCHAIRS01-TABLE_CHAIRS_36981</t>
+  </si>
+  <si>
+    <t>8685</t>
+  </si>
+  <si>
+    <t>2247</t>
+  </si>
+  <si>
+    <t>ITEM1482891117</t>
+  </si>
+  <si>
+    <t>5128</t>
+  </si>
+  <si>
+    <t>FIXTURESANDFITTINGS1-TABLESANDCHAIRS01-TABLE_CHAIRS_36981_AZENTMAIN_6001</t>
+  </si>
+  <si>
+    <t>5129</t>
+  </si>
+  <si>
+    <t>ITEM1032441445</t>
+  </si>
+  <si>
+    <t>5130</t>
+  </si>
+  <si>
+    <t>5131</t>
+  </si>
+  <si>
+    <t>5132</t>
+  </si>
+  <si>
+    <t>5133</t>
+  </si>
+  <si>
+    <t>ITEM1832431177</t>
+  </si>
+  <si>
+    <t>5134</t>
+  </si>
+  <si>
+    <t>5135</t>
+  </si>
+  <si>
+    <t>5136</t>
+  </si>
+  <si>
+    <t>ITEM1392971348</t>
+  </si>
+  <si>
+    <t>5137</t>
+  </si>
+  <si>
+    <t>114123</t>
+  </si>
+  <si>
+    <t>ITEM1032181133</t>
+  </si>
+  <si>
+    <t>5139</t>
+  </si>
+  <si>
+    <t>5140</t>
+  </si>
+  <si>
+    <t>5141</t>
+  </si>
+  <si>
+    <t>ITEM1272511249</t>
+  </si>
+  <si>
+    <t>5142</t>
+  </si>
+  <si>
+    <t>114128</t>
+  </si>
+  <si>
+    <t>5144</t>
+  </si>
+  <si>
+    <t>ITEM1642801022</t>
+  </si>
+  <si>
+    <t>5145</t>
+  </si>
+  <si>
+    <t>5146</t>
+  </si>
+  <si>
+    <t>5147</t>
+  </si>
+  <si>
+    <t>ITEM1712521451</t>
+  </si>
+  <si>
+    <t>5148</t>
+  </si>
+  <si>
+    <t>NITM181281</t>
+  </si>
+  <si>
+    <t>114134</t>
+  </si>
+  <si>
+    <t>5150</t>
+  </si>
+  <si>
+    <t>ITEM1142111389</t>
+  </si>
+  <si>
+    <t>5151</t>
+  </si>
+  <si>
+    <t>5152</t>
+  </si>
+  <si>
+    <t>5153</t>
+  </si>
+  <si>
+    <t>Table_Chairs491111</t>
+  </si>
+  <si>
+    <t>2567</t>
+  </si>
+  <si>
+    <t>01-001-Table_Chairs491111</t>
+  </si>
+  <si>
+    <t>8723</t>
+  </si>
+  <si>
+    <t>5168</t>
+  </si>
+  <si>
+    <t>5169</t>
+  </si>
+  <si>
+    <t>ITEM1892241448</t>
+  </si>
+  <si>
+    <t>5170</t>
+  </si>
+  <si>
+    <t>ITEM1932351487</t>
+  </si>
+  <si>
+    <t>5171</t>
+  </si>
+  <si>
+    <t>01-001-Table_Chairs491111_AZENTMAIN_1003</t>
+  </si>
+  <si>
+    <t>114155</t>
+  </si>
+  <si>
+    <t>ITEM1552961255</t>
+  </si>
+  <si>
+    <t>5173</t>
+  </si>
+  <si>
+    <t>114157</t>
+  </si>
+  <si>
+    <t>ITEM1812351489</t>
+  </si>
+  <si>
+    <t>5174</t>
+  </si>
+  <si>
+    <t>NITM165232</t>
+  </si>
+  <si>
+    <t>114159</t>
+  </si>
+  <si>
+    <t>Table_Chairs599</t>
+  </si>
+  <si>
+    <t>2568</t>
+  </si>
+  <si>
+    <t>01-001-Table_Chairs599</t>
+  </si>
+  <si>
+    <t>8731</t>
+  </si>
+  <si>
+    <t>2268</t>
+  </si>
+  <si>
+    <t>5176</t>
+  </si>
+  <si>
+    <t>5177</t>
+  </si>
+  <si>
+    <t>ITEM1522101452</t>
+  </si>
+  <si>
+    <t>5178</t>
+  </si>
+  <si>
+    <t>ITEM1632211451</t>
+  </si>
+  <si>
+    <t>5179</t>
+  </si>
+  <si>
+    <t>Table_Chairs512152</t>
+  </si>
+  <si>
+    <t>2569</t>
+  </si>
+  <si>
+    <t>01-001-Table_Chairs512152</t>
+  </si>
+  <si>
+    <t>8739</t>
+  </si>
+  <si>
+    <t>2269</t>
+  </si>
+  <si>
+    <t>5180</t>
+  </si>
+  <si>
+    <t>5181</t>
+  </si>
+  <si>
+    <t>ITEM1832261463</t>
+  </si>
+  <si>
+    <t>5182</t>
+  </si>
+  <si>
+    <t>ITEM1722091058</t>
+  </si>
+  <si>
+    <t>5183</t>
+  </si>
+  <si>
+    <t>01-001-Table_Chairs512152_AZENTMAIN_1003</t>
+  </si>
+  <si>
+    <t>114164</t>
+  </si>
+  <si>
+    <t>ITEM1522901263</t>
+  </si>
+  <si>
+    <t>5185</t>
+  </si>
+  <si>
+    <t>114166</t>
+  </si>
+  <si>
+    <t>ITEM1502091056</t>
+  </si>
+  <si>
+    <t>5186</t>
+  </si>
+  <si>
+    <t>NITM147202</t>
+  </si>
+  <si>
+    <t>114168</t>
   </si>
 </sst>
 </file>
@@ -5646,7 +6051,7 @@
     <col min="2" max="2" customWidth="true" style="10" width="61.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="10" width="12.5390625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="11.7578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="64.50390625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="63.38671875" collapsed="true"/>
     <col min="6" max="7" customWidth="true" style="10" width="50.0" collapsed="true"/>
     <col min="8" max="8" customWidth="true" style="10" width="56.714285714285715" collapsed="true"/>
     <col min="9" max="9" customWidth="true" style="10" width="96.85714285714286" collapsed="true"/>
@@ -5694,13 +6099,13 @@
         <v>296</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>1084</v>
+        <v>1519</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>1083</v>
+        <v>1518</v>
       </c>
       <c r="F2" s="15">
         <v>1001</v>
@@ -5726,13 +6131,13 @@
         <v>303</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>227</v>
+        <v>1404</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>228</v>
+        <v>1403</v>
       </c>
       <c r="F3" s="15">
         <v>2001</v>
@@ -5854,13 +6259,13 @@
         <v>309</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1346</v>
+        <v>1447</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>1345</v>
+        <v>1446</v>
       </c>
       <c r="F7" s="15">
         <v>6001</v>
@@ -6035,7 +6440,7 @@
     <col min="3" max="3" bestFit="true" customWidth="true" style="10" width="12.5390625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="11.7578125" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="10" width="62.714285714285715" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="64.50390625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="63.38671875" collapsed="true"/>
     <col min="7" max="8" customWidth="true" style="10" width="67.0" collapsed="true"/>
     <col min="9" max="10" customWidth="true" style="10" width="58.857142857142854" collapsed="true"/>
     <col min="11" max="11" customWidth="true" style="10" width="117.57142857142857" collapsed="true"/>
@@ -6128,7 +6533,7 @@
         <v>328</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>329</v>
+        <v>1521</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>56</v>
@@ -6137,7 +6542,7 @@
         <v>129</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>1083</v>
+        <v>1518</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>330</v>
@@ -6180,7 +6585,7 @@
         <v>338</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>339</v>
+        <v>1533</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>56</v>
@@ -6189,7 +6594,7 @@
         <v>129</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>1083</v>
+        <v>1518</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>340</v>
@@ -6203,7 +6608,7 @@
         <v>341</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>342</v>
+        <v>1532</v>
       </c>
       <c r="M3" s="15" t="s">
         <v>343</v>
@@ -6244,7 +6649,7 @@
         <v>345</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>346</v>
+        <v>1441</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>56</v>
@@ -6253,7 +6658,7 @@
         <v>129</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>228</v>
+        <v>1403</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>340</v>
@@ -6267,7 +6672,7 @@
         <v>341</v>
       </c>
       <c r="L4" s="14" t="s">
-        <v>347</v>
+        <v>1440</v>
       </c>
       <c r="M4" s="15" t="s">
         <v>343</v>
@@ -6500,7 +6905,7 @@
         <v>361</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1381</v>
+        <v>1483</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>56</v>
@@ -6509,7 +6914,7 @@
         <v>129</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>1345</v>
+        <v>1446</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>340</v>
@@ -6523,7 +6928,7 @@
         <v>341</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>1380</v>
+        <v>1482</v>
       </c>
       <c r="M8" s="15" t="s">
         <v>343</v>
@@ -6628,7 +7033,7 @@
         <v>368</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1086</v>
+        <v>1522</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>56</v>
@@ -6637,7 +7042,7 @@
         <v>129</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>1083</v>
+        <v>1518</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>340</v>
@@ -6833,7 +7238,7 @@
     <col min="2" max="2" customWidth="true" style="10" width="68.85714285714286" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="10" width="12.5390625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="11.7578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="82.15234375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="81.03515625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="17.35546875" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="10" width="68.85714285714286" collapsed="true"/>
     <col min="8" max="8" customWidth="true" style="10" width="57.57142857142857" collapsed="true"/>
@@ -6893,16 +7298,16 @@
         <v>378</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>379</v>
+        <v>1528</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>380</v>
+        <v>1527</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>381</v>
+        <v>1525</v>
       </c>
       <c r="G2" s="15">
         <v>100000000</v>
@@ -6934,16 +7339,16 @@
         <v>388</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>389</v>
+        <v>1531</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>380</v>
+        <v>1527</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>390</v>
+        <v>1529</v>
       </c>
       <c r="G3" s="15">
         <v>10000</v>
@@ -6975,16 +7380,16 @@
         <v>392</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>393</v>
+        <v>1438</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>394</v>
+        <v>1408</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>395</v>
+        <v>1436</v>
       </c>
       <c r="G4" s="15">
         <v>10000</v>
@@ -7016,16 +7421,16 @@
         <v>396</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1369</v>
+        <v>1471</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>1367</v>
+        <v>1469</v>
       </c>
       <c r="G5" s="15">
         <v>10000</v>
@@ -7308,7 +7713,7 @@
     <col min="2" max="2" customWidth="true" style="10" width="64.28571428571429" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="10" width="12.5390625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="11.7578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="82.15234375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="81.03515625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="17.35546875" collapsed="true"/>
     <col min="7" max="8" customWidth="true" style="10" width="59.0" collapsed="true"/>
     <col min="9" max="9" customWidth="true" style="10" width="93.14285714285714" collapsed="true"/>
@@ -7492,16 +7897,16 @@
         <v>430</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>431</v>
+        <v>1416</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>394</v>
+        <v>1408</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>432</v>
+        <v>1414</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>382</v>
@@ -7562,16 +7967,16 @@
         <v>437</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>1354</v>
+        <v>1455</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>1352</v>
+        <v>1453</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>382</v>
@@ -7877,7 +8282,7 @@
     <col min="2" max="2" customWidth="true" style="10" width="68.85714285714286" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="10" width="12.5390625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="11.7578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="82.15234375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="81.03515625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="17.35546875" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="10" width="59.42857142857143" collapsed="true"/>
     <col min="8" max="8" customWidth="true" style="10" width="107.0" collapsed="true"/>
@@ -7958,16 +8363,16 @@
         <v>468</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>469</v>
+        <v>1417</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>394</v>
+        <v>1408</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>432</v>
+        <v>1414</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>464</v>
@@ -8022,16 +8427,16 @@
         <v>472</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1355</v>
+        <v>1456</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>1352</v>
+        <v>1453</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>464</v>
@@ -8277,7 +8682,7 @@
     <col min="2" max="2" customWidth="true" style="10" width="65.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="10" width="12.5390625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="11.7578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="82.15234375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="81.03515625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="17.35546875" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="10" width="56.714285714285715" collapsed="true"/>
     <col min="8" max="8" customWidth="true" style="10" width="110.85714285714286" collapsed="true"/>
@@ -8464,10 +8869,10 @@
         <v>56</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>1108</v>
+        <v>1527</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>1123</v>
+        <v>1534</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>491</v>
@@ -8557,16 +8962,16 @@
         <v>516</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>517</v>
+        <v>1434</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>394</v>
+        <v>1408</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>518</v>
+        <v>1432</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>491</v>
@@ -8590,16 +8995,16 @@
         <v>519</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1373</v>
+        <v>1475</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>1371</v>
+        <v>1473</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>491</v>
@@ -8812,7 +9217,7 @@
     <col min="2" max="2" customWidth="true" style="10" width="80.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="10" width="12.5390625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="11.7578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="82.15234375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="81.03515625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="17.35546875" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="10" width="32.42857142857143" collapsed="true"/>
     <col min="8" max="8" customWidth="true" style="10" width="105.57142857142857" collapsed="true"/>
@@ -8861,16 +9266,16 @@
         <v>531</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>532</v>
+        <v>1409</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>394</v>
+        <v>1408</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>347</v>
+        <v>1440</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>533</v>
@@ -8893,16 +9298,16 @@
         <v>538</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>539</v>
+        <v>1413</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>394</v>
+        <v>1408</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>540</v>
+        <v>1410</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>533</v>
@@ -8925,16 +9330,16 @@
         <v>542</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>543</v>
+        <v>1418</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>394</v>
+        <v>1408</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>432</v>
+        <v>1414</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>533</v>
@@ -8957,16 +9362,16 @@
         <v>545</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>546</v>
+        <v>1422</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>394</v>
+        <v>1408</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>547</v>
+        <v>1419</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>533</v>
@@ -8989,16 +9394,16 @@
         <v>549</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>550</v>
+        <v>1426</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>394</v>
+        <v>1408</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>551</v>
+        <v>1423</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>533</v>
@@ -9021,16 +9426,16 @@
         <v>553</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>554</v>
+        <v>1431</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>394</v>
+        <v>1408</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>555</v>
+        <v>1427</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>533</v>
@@ -9053,16 +9458,16 @@
         <v>557</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>558</v>
+        <v>1435</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>394</v>
+        <v>1408</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>518</v>
+        <v>1432</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>533</v>
@@ -9085,16 +9490,16 @@
         <v>560</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>561</v>
+        <v>1439</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>394</v>
+        <v>1408</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>395</v>
+        <v>1436</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>533</v>
@@ -9117,16 +9522,16 @@
         <v>563</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>564</v>
+        <v>1443</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>1380</v>
+        <v>1482</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>533</v>
@@ -9181,16 +9586,16 @@
         <v>567</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>1362</v>
+        <v>1464</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>1360</v>
+        <v>1462</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>533</v>
@@ -9436,7 +9841,7 @@
     <col min="2" max="2" customWidth="true" style="10" width="60.285714285714285" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="10" width="12.5390625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="11.7578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="82.15234375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="81.03515625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="17.35546875" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="10" width="39.71875" collapsed="true"/>
     <col min="8" max="8" customWidth="true" style="10" width="39.285714285714285" collapsed="true"/>
@@ -9756,16 +10161,16 @@
         <v>615</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>616</v>
+        <v>1425</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>394</v>
+        <v>1408</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>551</v>
+        <v>1423</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>593</v>
@@ -9909,16 +10314,16 @@
         <v>621</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1365</v>
+        <v>1467</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>1363</v>
+        <v>1465</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>593</v>
@@ -10199,7 +10604,7 @@
     <col min="2" max="2" customWidth="true" style="10" width="68.85714285714286" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="10" width="12.5390625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="11.7578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="82.15234375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="81.03515625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="17.35546875" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="10" width="32.8828125" collapsed="true"/>
     <col min="8" max="8" customWidth="true" style="10" width="37.42857142857143" collapsed="true"/>
@@ -10260,16 +10665,16 @@
         <v>637</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>1351</v>
+        <v>1460</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>1357</v>
+        <v>1458</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>640</v>
@@ -10298,16 +10703,16 @@
         <v>646</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>647</v>
+        <v>1421</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>394</v>
+        <v>1408</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>547</v>
+        <v>1419</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>640</v>
@@ -10641,16 +11046,16 @@
         <v>665</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>1356</v>
+        <v>1457</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>1352</v>
+        <v>1453</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>640</v>
@@ -10679,16 +11084,16 @@
         <v>668</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>1385</v>
+        <v>1461</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>1357</v>
+        <v>1458</v>
       </c>
       <c r="G14" s="14" t="s">
         <v>670</v>
@@ -10719,10 +11124,10 @@
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>1360</v>
+        <v>1462</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="15" t="s">
@@ -10749,16 +11154,16 @@
         <v>675</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>1366</v>
+        <v>1468</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>1363</v>
+        <v>1465</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>640</v>
@@ -10787,16 +11192,16 @@
         <v>678</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>1383</v>
+        <v>1485</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>1380</v>
+        <v>1482</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>640</v>
@@ -10825,16 +11230,16 @@
         <v>681</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>1370</v>
+        <v>1472</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>1367</v>
+        <v>1469</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>640</v>
@@ -10863,16 +11268,16 @@
         <v>684</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>1374</v>
+        <v>1476</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>1371</v>
+        <v>1473</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>640</v>
@@ -10901,16 +11306,16 @@
         <v>687</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>1379</v>
+        <v>1481</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>1377</v>
+        <v>1479</v>
       </c>
       <c r="G20" s="14" t="s">
         <v>640</v>
@@ -10951,7 +11356,7 @@
     <col min="2" max="2" customWidth="true" style="10" width="60.285714285714285" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="10" width="12.5390625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="11.7578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="82.15234375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="81.03515625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="17.35546875" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="10" width="36.0" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="10" width="24.3828125" collapsed="true"/>
@@ -11012,22 +11417,22 @@
         <v>694</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>695</v>
+        <v>1535</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>380</v>
+        <v>1527</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>696</v>
+        <v>1532</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>697</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>698</v>
+        <v>1534</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>699</v>
@@ -11053,22 +11458,22 @@
         <v>704</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>705</v>
+        <v>1430</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>394</v>
+        <v>1408</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>555</v>
+        <v>1427</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>697</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>706</v>
+        <v>1429</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>699</v>
@@ -11135,22 +11540,22 @@
         <v>710</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>1378</v>
+        <v>1480</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>1375</v>
+        <v>1477</v>
       </c>
       <c r="G5" s="15" t="s">
         <v>697</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>1377</v>
+        <v>1479</v>
       </c>
       <c r="I5" s="15" t="s">
         <v>699</v>
@@ -11584,7 +11989,7 @@
     <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="12.875" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="12.875" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="12.875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="10" width="82.15234375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="10" width="81.03515625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" style="10" width="17.35546875" collapsed="true"/>
     <col min="9" max="9" customWidth="true" style="10" width="41.42857142857143" collapsed="true"/>
     <col min="10" max="10" customWidth="true" style="10" width="61.857142857142854" collapsed="true"/>
@@ -11966,7 +12371,7 @@
         <v>771</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>772</v>
+        <v>1442</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>37</v>
@@ -11974,10 +12379,10 @@
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14" t="s">
-        <v>394</v>
+        <v>1408</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>347</v>
+        <v>1440</v>
       </c>
       <c r="I9" s="17" t="s">
         <v>773</v>
@@ -12009,22 +12414,22 @@
         <v>774</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>1382</v>
+        <v>1484</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>37</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>37</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>1350</v>
+        <v>1451</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>1380</v>
+        <v>1482</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>776</v>
@@ -34176,7 +34581,7 @@
         <v>162</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>1082</v>
+        <v>1517</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>56</v>
@@ -34191,7 +34596,7 @@
         <v>165</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>1081</v>
+        <v>1516</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>167</v>
@@ -34217,7 +34622,7 @@
         <v>172</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>1400</v>
+        <v>1402</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>56</v>
@@ -34232,7 +34637,7 @@
         <v>176</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>1399</v>
+        <v>1401</v>
       </c>
       <c r="I3" s="25" t="s">
         <v>178</v>
@@ -34381,7 +34786,7 @@
         <v>197</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1344</v>
+        <v>1445</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>56</v>
@@ -34396,7 +34801,7 @@
         <v>176</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>1343</v>
+        <v>1444</v>
       </c>
       <c r="I7" s="15" t="s">
         <v>188</v>
@@ -34632,7 +35037,7 @@
     <col min="2" max="2" customWidth="true" style="10" width="59.42857142857143" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="10" width="12.5390625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="11.7578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="64.50390625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="63.38671875" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="10" width="55.857142857142854" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="10" width="50.714285714285715" collapsed="true"/>
     <col min="8" max="8" customWidth="true" style="10" width="26.285714285714285" collapsed="true"/>
@@ -34700,13 +35105,13 @@
         <v>215</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>1084</v>
+        <v>1519</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>1083</v>
+        <v>1518</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>218</v>
@@ -34747,13 +35152,13 @@
         <v>226</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>227</v>
+        <v>1404</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>228</v>
+        <v>1403</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>229</v>
@@ -34935,13 +35340,13 @@
         <v>243</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1346</v>
+        <v>1447</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>1345</v>
+        <v>1446</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>218</v>
@@ -35222,7 +35627,7 @@
     <col min="2" max="2" customWidth="true" style="10" width="71.14285714285714" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" style="10" width="12.5390625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="11.7578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="64.50390625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="63.38671875" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="10" width="80.71428571428571" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="10" width="78.57142857142857" collapsed="true"/>
     <col min="8" max="8" customWidth="true" style="10" width="81.42857142857143" collapsed="true"/>
@@ -35303,13 +35708,13 @@
         <v>263</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>1085</v>
+        <v>1520</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>1083</v>
+        <v>1518</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>265</v>
@@ -35359,13 +35764,13 @@
         <v>270</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>271</v>
+        <v>1405</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>228</v>
+        <v>1403</v>
       </c>
       <c r="F3" s="17" t="s">
         <v>272</v>
@@ -35583,13 +35988,13 @@
         <v>282</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>1347</v>
+        <v>1448</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>1345</v>
+        <v>1446</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>284</v>

</xml_diff>